<commit_message>
will search through 1 excel sheet sheet and return if value was found or not
</commit_message>
<xml_diff>
--- a/Shipping Book with RFID.xlsx
+++ b/Shipping Book with RFID.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f0af74de07732f5/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krith\huskiesInvent\HuskiesInventTeam5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E28FC63D-5CD0-4E3E-B093-C93DDF2BC3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC06F22-6AF5-49F7-BAC4-2DBFCE56222A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DD0E8133-3D0B-4E84-9D61-459F2CA97A73}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{DD0E8133-3D0B-4E84-9D61-459F2CA97A73}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Pkg Line No</t>
   </si>
   <si>
-    <t>RFID Number</t>
-  </si>
-  <si>
     <t xml:space="preserve">S253441 </t>
   </si>
   <si>
@@ -108,13 +105,16 @@
   </si>
   <si>
     <t>E2004704D9C06026AB7F0114</t>
+  </si>
+  <si>
+    <t>RFIDNumber</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,19 +494,19 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" customWidth="1"/>
+    <col min="4" max="4" width="29.26953125" customWidth="1"/>
+    <col min="5" max="5" width="30.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -517,12 +517,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -531,12 +531,12 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
-      <c r="A3" t="s">
-        <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -545,12 +545,12 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -559,12 +559,12 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15">
-      <c r="A5" t="s">
-        <v>10</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -573,12 +573,12 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15">
-      <c r="A6" t="s">
-        <v>12</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -587,12 +587,12 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="15">
-      <c r="A7" t="s">
-        <v>14</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -601,12 +601,12 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15">
-      <c r="A8" t="s">
-        <v>16</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -615,12 +615,12 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15">
-      <c r="A9" t="s">
-        <v>18</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -629,12 +629,12 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="15">
-      <c r="A10" t="s">
-        <v>20</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -643,12 +643,12 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15">
-      <c r="A11" t="s">
-        <v>22</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -657,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>